<commit_message>
MergeTables.py gemaakt die Conditions_table.xlsx met experiment_table.csv fuseert
Signed-off-by: Housermans <mahuismans@gmail.com>
</commit_message>
<xml_diff>
--- a/input/Conditions_table.xlsx
+++ b/input/Conditions_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhuismans/PycharmProjects/E21-002_drugscreen/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231304A7-49B4-B347-B704-11A6602DC4B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26AAE109-9C55-2142-8CDD-804EEC41B603}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="2400" windowWidth="21040" windowHeight="16940" xr2:uid="{F7AF2FA9-ECF8-7442-9F67-4D629195362E}"/>
+    <workbookView xWindow="1640" yWindow="500" windowWidth="25400" windowHeight="16940" xr2:uid="{F7AF2FA9-ECF8-7442-9F67-4D629195362E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -147,8 +147,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3F0385-C9A5-0F43-8FE6-79160C0A2D8B}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="A1:R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,46 +535,46 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>128</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2">
-        <v>16</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
       <c r="I2">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -588,69 +591,69 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F3">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>10000</v>
+        <v>5</v>
       </c>
       <c r="I3">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
+      <c r="P3" s="1">
+        <v>0.11903712</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0.11903712</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -662,16 +665,16 @@
         <v>16</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -700,13 +703,13 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -756,16 +759,16 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
@@ -789,13 +792,13 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -812,16 +815,16 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
@@ -844,14 +847,14 @@
       <c r="K7">
         <v>0</v>
       </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
+      <c r="L7" s="1">
+        <v>0.11903712</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.11903712</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -868,16 +871,16 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
@@ -901,13 +904,13 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -924,22 +927,22 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
       </c>
       <c r="F9">
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -954,16 +957,16 @@
         <v>8</v>
       </c>
       <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>5</v>
-      </c>
-      <c r="M9">
-        <v>20000</v>
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.11903712</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0.11903712</v>
       </c>
       <c r="N9">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -980,22 +983,22 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
       <c r="F10">
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1010,25 +1013,25 @@
         <v>8</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>5</v>
+        <v>175</v>
       </c>
       <c r="M10">
-        <v>20000</v>
+        <v>175</v>
       </c>
       <c r="N10">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10">
-        <v>120</v>
+        <v>175</v>
       </c>
       <c r="Q10">
-        <v>120</v>
+        <v>175</v>
       </c>
       <c r="R10">
         <v>1</v>
@@ -1036,13 +1039,13 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
@@ -1056,11 +1059,11 @@
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11">
-        <v>120</v>
-      </c>
-      <c r="I11">
-        <v>120</v>
+      <c r="H11" s="1">
+        <v>10.0189576</v>
+      </c>
+      <c r="I11" s="1">
+        <v>10.0189576</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1092,61 +1095,65 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F12">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>5</v>
-      </c>
-      <c r="I12">
-        <v>20000</v>
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.119037158575</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.119037158575</v>
       </c>
       <c r="J12">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="R12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R12">
+    <sortCondition descending="1" ref="F2:F12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>